<commit_message>
se agregan nuevos campos
</commit_message>
<xml_diff>
--- a/templates/11.11.25.xlsx
+++ b/templates/11.11.25.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indicaciones_medicas2\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\indicaciones_medicas\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D65552B-60E5-4BA7-BA2C-346061486534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E870FE50-828D-4BDD-89EF-6185FA8A086D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8F26B026-E952-45BF-A1DB-55563CFCC2D9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F26B026-E952-45BF-A1DB-55563CFCC2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicaciones médicas" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="113">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -364,6 +364,24 @@
   </si>
   <si>
     <t>TOF 1-2 de 4</t>
+  </si>
+  <si>
+    <t>{{FLEBOS}}</t>
+  </si>
+  <si>
+    <t>FLEBOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{DOSIS}} </t>
+  </si>
+  <si>
+    <t>{{intervalo}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/  / </t>
+  </si>
+  <si>
+    <t>{{Via}}</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1046,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
@@ -1290,6 +1308,16 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1299,89 +1327,101 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1398,8 +1438,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1413,10 +1451,14 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1428,99 +1470,94 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1588,24 +1625,11 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Estilo 1" xfId="2" xr:uid="{5A164531-6111-430B-BEE7-AD80169FE218}"/>
@@ -1967,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F7F867-996E-4386-BA02-4186311E04F2}">
-  <dimension ref="A1:Q112"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,13 +2037,13 @@
     <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -2034,12 +2058,12 @@
     <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="166" t="s">
+      <c r="C3" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
       <c r="G3" s="12"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -2118,10 +2142,10 @@
       <c r="I6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="169"/>
+      <c r="K6" s="137"/>
       <c r="L6" s="56" t="s">
         <v>8</v>
       </c>
@@ -2131,48 +2155,48 @@
       <c r="N6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="170" t="s">
+      <c r="O6" s="138" t="s">
         <v>50</v>
       </c>
-      <c r="P6" s="171"/>
+      <c r="P6" s="139"/>
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="132"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="142"/>
       <c r="I7" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="180" t="s">
+      <c r="J7" s="152" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="140"/>
+      <c r="K7" s="153"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="144"/>
       <c r="N7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="173" t="s">
+      <c r="O7" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="P7" s="140"/>
+      <c r="P7" s="144"/>
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="174" t="s">
+      <c r="A8" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="175"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
@@ -2185,91 +2209,91 @@
       <c r="F8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="176" t="s">
+      <c r="G8" s="147" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="177"/>
-      <c r="I8" s="141" t="s">
+      <c r="H8" s="148"/>
+      <c r="I8" s="149" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="140"/>
+      <c r="J8" s="144"/>
       <c r="K8" s="59" t="s">
         <v>57</v>
       </c>
       <c r="L8" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="M8" s="178" t="s">
+      <c r="M8" s="150" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="169"/>
-      <c r="O8" s="169"/>
-      <c r="P8" s="179"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="151"/>
       <c r="Q8" s="63"/>
     </row>
     <row r="9" spans="1:17" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="139" t="s">
+      <c r="A9" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="140"/>
-      <c r="C9" s="150" t="s">
+      <c r="B9" s="144"/>
+      <c r="C9" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="143"/>
-      <c r="E9" s="143"/>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="143"/>
-      <c r="I9" s="143"/>
-      <c r="J9" s="143"/>
-      <c r="K9" s="143"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="141"/>
+      <c r="K9" s="141"/>
       <c r="L9" s="67"/>
-      <c r="M9" s="151"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="130"/>
-      <c r="P9" s="140"/>
+      <c r="M9" s="161"/>
+      <c r="N9" s="153"/>
+      <c r="O9" s="153"/>
+      <c r="P9" s="144"/>
       <c r="Q9" s="64"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="141" t="s">
+      <c r="A10" s="149" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="140"/>
-      <c r="C10" s="142" t="s">
+      <c r="B10" s="144"/>
+      <c r="C10" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="143"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="143"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="143"/>
-      <c r="K10" s="143"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="143"/>
-      <c r="N10" s="143"/>
-      <c r="O10" s="143"/>
-      <c r="P10" s="132"/>
+      <c r="D10" s="141"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="141"/>
+      <c r="G10" s="141"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
+      <c r="J10" s="141"/>
+      <c r="K10" s="141"/>
+      <c r="L10" s="141"/>
+      <c r="M10" s="141"/>
+      <c r="N10" s="141"/>
+      <c r="O10" s="141"/>
+      <c r="P10" s="142"/>
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="156" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="145"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="146" t="s">
+      <c r="D11" s="158" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="145"/>
+      <c r="E11" s="157"/>
       <c r="F11" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="129"/>
-      <c r="H11" s="130"/>
+      <c r="G11" s="183"/>
+      <c r="H11" s="153"/>
       <c r="I11" s="74"/>
       <c r="J11" s="69" t="s">
         <v>26</v>
@@ -2286,15 +2310,15 @@
       <c r="N11" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="131" t="s">
+      <c r="O11" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="P11" s="132"/>
+      <c r="P11" s="142"/>
       <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
+      <c r="A12" s="185"/>
+      <c r="B12" s="186"/>
       <c r="C12" s="78" t="s">
         <v>104</v>
       </c>
@@ -2324,16 +2348,16 @@
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
-      <c r="G13" s="147"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="149"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="125"/>
+      <c r="K13" s="125"/>
+      <c r="L13" s="125"/>
+      <c r="M13" s="125"/>
+      <c r="N13" s="125"/>
+      <c r="O13" s="125"/>
+      <c r="P13" s="126"/>
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -2341,22 +2365,22 @@
       <c r="B14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="128" t="s">
+      <c r="C14" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="126"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="126"/>
-      <c r="P14" s="127"/>
+      <c r="D14" s="171"/>
+      <c r="E14" s="171"/>
+      <c r="F14" s="171"/>
+      <c r="G14" s="171"/>
+      <c r="H14" s="171"/>
+      <c r="I14" s="171"/>
+      <c r="J14" s="171"/>
+      <c r="K14" s="171"/>
+      <c r="L14" s="171"/>
+      <c r="M14" s="171"/>
+      <c r="N14" s="171"/>
+      <c r="O14" s="171"/>
+      <c r="P14" s="173"/>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -2401,12 +2425,12 @@
       <c r="B16" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="187" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="136"/>
-      <c r="E16" s="136"/>
-      <c r="F16" s="137"/>
+      <c r="D16" s="188"/>
+      <c r="E16" s="188"/>
+      <c r="F16" s="189"/>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
       <c r="I16" s="50" t="s">
@@ -2423,245 +2447,254 @@
       <c r="P16" s="62"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="119"/>
       <c r="B17" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="138" t="s">
+      <c r="C17" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="136"/>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
-      <c r="O17" s="136"/>
-      <c r="P17" s="137"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="184"/>
-      <c r="B18" s="118" t="s">
+      <c r="D17" s="188"/>
+      <c r="E17" s="188"/>
+      <c r="F17" s="188"/>
+      <c r="G17" s="188"/>
+      <c r="H17" s="188"/>
+      <c r="I17" s="188"/>
+      <c r="J17" s="188"/>
+      <c r="K17" s="188"/>
+      <c r="L17" s="188"/>
+      <c r="M17" s="188"/>
+      <c r="N17" s="188"/>
+      <c r="O17" s="188"/>
+      <c r="P17" s="189"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="120"/>
+      <c r="B18" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="119"/>
-      <c r="O18" s="119"/>
-      <c r="P18" s="120"/>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="132"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="132"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="132"/>
+      <c r="L18" s="132"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="133"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="179" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="124"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="122"/>
-      <c r="K19" s="122"/>
-      <c r="L19" s="122"/>
-      <c r="M19" s="122"/>
-      <c r="N19" s="122"/>
-      <c r="O19" s="122"/>
-      <c r="P19" s="123"/>
-    </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="166"/>
+      <c r="G19" s="180"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
+      <c r="O19" s="165"/>
+      <c r="P19" s="166"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="126"/>
-      <c r="I20" s="126"/>
-      <c r="J20" s="126"/>
-      <c r="K20" s="126"/>
-      <c r="L20" s="126"/>
-      <c r="M20" s="126"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="126"/>
-      <c r="P20" s="127"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="181"/>
+      <c r="C20" s="171"/>
+      <c r="D20" s="171"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="171"/>
+      <c r="H20" s="171"/>
+      <c r="I20" s="171"/>
+      <c r="J20" s="171"/>
+      <c r="K20" s="171"/>
+      <c r="L20" s="171"/>
+      <c r="M20" s="171"/>
+      <c r="N20" s="171"/>
+      <c r="O20" s="171"/>
+      <c r="P20" s="173"/>
+      <c r="S20" s="174" t="s">
+        <v>111</v>
+      </c>
+      <c r="T20" s="114"/>
+      <c r="U20" s="115"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="152" t="s">
+      <c r="B21" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="148"/>
-      <c r="K21" s="148"/>
-      <c r="L21" s="148"/>
-      <c r="M21" s="148"/>
-      <c r="N21" s="148"/>
-      <c r="O21" s="148"/>
-      <c r="P21" s="149"/>
-    </row>
-    <row r="22" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="125"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="126"/>
+    </row>
+    <row r="22" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="153" t="s">
+      <c r="B22" s="163" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="154"/>
-      <c r="D22" s="154"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="122"/>
-      <c r="I22" s="122"/>
-      <c r="J22" s="122"/>
-      <c r="K22" s="122"/>
-      <c r="L22" s="122"/>
-      <c r="M22" s="122"/>
-      <c r="N22" s="122"/>
-      <c r="O22" s="122"/>
-      <c r="P22" s="123"/>
-    </row>
-    <row r="23" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="122"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="165"/>
+      <c r="I22" s="165"/>
+      <c r="J22" s="165"/>
+      <c r="K22" s="165"/>
+      <c r="L22" s="165"/>
+      <c r="M22" s="165"/>
+      <c r="N22" s="165"/>
+      <c r="O22" s="165"/>
+      <c r="P22" s="166"/>
+    </row>
+    <row r="23" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="157" t="s">
+      <c r="B23" s="167" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="158"/>
-      <c r="D23" s="158"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="216" t="s">
+      <c r="C23" s="168"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="175" t="s">
         <v>105</v>
       </c>
-      <c r="H23" s="165"/>
+      <c r="H23" s="177"/>
       <c r="I23" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="J23" s="218"/>
-      <c r="K23" s="216" t="s">
+      <c r="J23" s="112"/>
+      <c r="K23" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="217"/>
+      <c r="L23" s="176"/>
       <c r="M23" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="165"/>
-      <c r="O23" s="143"/>
-      <c r="P23" s="132"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="185"/>
-      <c r="B24" s="160"/>
-      <c r="C24" s="126"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="162"/>
-      <c r="H24" s="162"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="162"/>
-      <c r="K24" s="126"/>
-      <c r="L24" s="126"/>
-      <c r="M24" s="126"/>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
-      <c r="P24" s="127"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="184"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="162"/>
-      <c r="D25" s="162"/>
-      <c r="E25" s="162"/>
-      <c r="F25" s="162"/>
-      <c r="G25" s="162"/>
-      <c r="H25" s="162"/>
-      <c r="I25" s="162"/>
-      <c r="J25" s="162"/>
-      <c r="K25" s="162"/>
-      <c r="L25" s="162"/>
-      <c r="M25" s="162"/>
-      <c r="N25" s="162"/>
-      <c r="O25" s="162"/>
-      <c r="P25" s="163"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N23" s="177"/>
+      <c r="O23" s="141"/>
+      <c r="P23" s="142"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="171"/>
+      <c r="D24" s="171"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="171"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="171"/>
+      <c r="L24" s="171"/>
+      <c r="M24" s="171"/>
+      <c r="N24" s="171"/>
+      <c r="O24" s="171"/>
+      <c r="P24" s="173"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="191" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="192"/>
+      <c r="D25" s="192"/>
+      <c r="E25" s="193"/>
+      <c r="F25" s="193"/>
+      <c r="G25" s="193"/>
+      <c r="H25" s="193"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="193"/>
+      <c r="K25" s="193"/>
+      <c r="L25" s="193"/>
+      <c r="M25" s="193"/>
+      <c r="N25" s="193"/>
+      <c r="O25" s="193"/>
+      <c r="P25" s="193"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
-      <c r="B26" s="186" t="s">
+      <c r="B26" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="154"/>
-      <c r="D26" s="154"/>
-      <c r="E26" s="154"/>
-      <c r="F26" s="155"/>
-      <c r="G26" s="188"/>
-      <c r="H26" s="167"/>
-      <c r="I26" s="167"/>
-      <c r="J26" s="167"/>
-      <c r="K26" s="167"/>
-      <c r="L26" s="167"/>
-      <c r="M26" s="167"/>
-      <c r="N26" s="167"/>
-      <c r="O26" s="167"/>
-      <c r="P26" s="189"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
+      <c r="N26" s="128"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="129"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
-      <c r="B27" s="187"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="190"/>
-      <c r="H27" s="167"/>
-      <c r="I27" s="167"/>
-      <c r="J27" s="167"/>
-      <c r="K27" s="167"/>
-      <c r="L27" s="167"/>
-      <c r="M27" s="167"/>
-      <c r="N27" s="167"/>
-      <c r="O27" s="167"/>
-      <c r="P27" s="189"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="124"/>
+      <c r="C27" s="125"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="125"/>
+      <c r="F27" s="126"/>
+      <c r="G27" s="130"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="128"/>
+      <c r="O27" s="128"/>
+      <c r="P27" s="129"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="113"/>
-      <c r="D28" s="114"/>
+      <c r="B28" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118"/>
       <c r="E28" s="42"/>
       <c r="F28" s="43"/>
       <c r="G28" s="44"/>
@@ -2675,15 +2708,19 @@
       <c r="O28" s="44"/>
       <c r="P28" s="43"/>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="164" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117"/>
+      <c r="B29" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E29" s="45"/>
       <c r="F29" s="45"/>
       <c r="G29" s="46"/>
@@ -2697,15 +2734,15 @@
       <c r="O29" s="47"/>
       <c r="P29" s="47"/>
     </row>
-    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="113"/>
-      <c r="D30" s="114"/>
+      <c r="B30" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="117"/>
+      <c r="D30" s="118"/>
       <c r="E30" s="48"/>
       <c r="F30" s="49"/>
       <c r="G30" s="50"/>
@@ -2719,15 +2756,19 @@
       <c r="O30" s="34"/>
       <c r="P30" s="34"/>
     </row>
-    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="116"/>
-      <c r="D31" s="117"/>
+      <c r="B31" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E31" s="51"/>
       <c r="F31" s="45"/>
       <c r="G31" s="46"/>
@@ -2741,15 +2782,15 @@
       <c r="O31" s="47"/>
       <c r="P31" s="47"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="113"/>
-      <c r="D32" s="114"/>
+      <c r="B32" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="117"/>
+      <c r="D32" s="118"/>
       <c r="E32" s="48"/>
       <c r="F32" s="49"/>
       <c r="G32" s="50"/>
@@ -2767,11 +2808,15 @@
       <c r="A33" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="116"/>
-      <c r="D33" s="117"/>
+      <c r="B33" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E33" s="51"/>
       <c r="F33" s="45"/>
       <c r="G33" s="46"/>
@@ -2789,11 +2834,11 @@
       <c r="A34" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="113"/>
-      <c r="D34" s="114"/>
+      <c r="B34" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="117"/>
+      <c r="D34" s="118"/>
       <c r="E34" s="48"/>
       <c r="F34" s="49"/>
       <c r="G34" s="50"/>
@@ -2811,11 +2856,15 @@
       <c r="A35" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="116"/>
-      <c r="D35" s="117"/>
+      <c r="B35" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E35" s="51"/>
       <c r="F35" s="45"/>
       <c r="G35" s="46"/>
@@ -2833,11 +2882,11 @@
       <c r="A36" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="113"/>
-      <c r="D36" s="114"/>
+      <c r="B36" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="117"/>
+      <c r="D36" s="118"/>
       <c r="E36" s="48"/>
       <c r="F36" s="49"/>
       <c r="G36" s="50"/>
@@ -2855,11 +2904,15 @@
       <c r="A37" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="116"/>
-      <c r="D37" s="117"/>
+      <c r="B37" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E37" s="51"/>
       <c r="F37" s="45"/>
       <c r="G37" s="46"/>
@@ -2877,11 +2930,11 @@
       <c r="A38" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="113"/>
-      <c r="D38" s="114"/>
+      <c r="B38" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="117"/>
+      <c r="D38" s="118"/>
       <c r="E38" s="48"/>
       <c r="F38" s="49"/>
       <c r="G38" s="50"/>
@@ -2899,11 +2952,15 @@
       <c r="A39" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="116"/>
-      <c r="D39" s="117"/>
+      <c r="B39" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E39" s="51"/>
       <c r="F39" s="45"/>
       <c r="G39" s="46"/>
@@ -2921,11 +2978,11 @@
       <c r="A40" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="113"/>
-      <c r="D40" s="114"/>
+      <c r="B40" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="117"/>
+      <c r="D40" s="118"/>
       <c r="E40" s="48"/>
       <c r="F40" s="49"/>
       <c r="G40" s="50"/>
@@ -2943,11 +3000,15 @@
       <c r="A41" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="116"/>
-      <c r="D41" s="117"/>
+      <c r="B41" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E41" s="51"/>
       <c r="F41" s="45"/>
       <c r="G41" s="46"/>
@@ -2965,11 +3026,11 @@
       <c r="A42" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="113"/>
-      <c r="D42" s="114"/>
+      <c r="B42" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="117"/>
+      <c r="D42" s="118"/>
       <c r="E42" s="48"/>
       <c r="F42" s="49"/>
       <c r="G42" s="50"/>
@@ -2987,11 +3048,15 @@
       <c r="A43" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="116"/>
-      <c r="D43" s="117"/>
+      <c r="B43" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E43" s="51"/>
       <c r="F43" s="45"/>
       <c r="G43" s="46"/>
@@ -3009,11 +3074,11 @@
       <c r="A44" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="113"/>
-      <c r="D44" s="114"/>
+      <c r="B44" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="117"/>
+      <c r="D44" s="118"/>
       <c r="E44" s="48"/>
       <c r="F44" s="49"/>
       <c r="G44" s="50"/>
@@ -3031,11 +3096,15 @@
       <c r="A45" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="116"/>
-      <c r="D45" s="117"/>
+      <c r="B45" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E45" s="51"/>
       <c r="F45" s="45"/>
       <c r="G45" s="46"/>
@@ -3053,11 +3122,11 @@
       <c r="A46" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="113"/>
-      <c r="D46" s="114"/>
+      <c r="B46" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="117"/>
+      <c r="D46" s="118"/>
       <c r="E46" s="48"/>
       <c r="F46" s="49"/>
       <c r="G46" s="50"/>
@@ -3075,11 +3144,15 @@
       <c r="A47" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="116"/>
-      <c r="D47" s="117"/>
+      <c r="B47" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E47" s="51"/>
       <c r="F47" s="45"/>
       <c r="G47" s="46"/>
@@ -3097,11 +3170,11 @@
       <c r="A48" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="114"/>
+      <c r="B48" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="117"/>
+      <c r="D48" s="118"/>
       <c r="E48" s="48"/>
       <c r="F48" s="49"/>
       <c r="G48" s="50"/>
@@ -3119,11 +3192,15 @@
       <c r="A49" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="116"/>
-      <c r="D49" s="117"/>
+      <c r="B49" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E49" s="51"/>
       <c r="F49" s="45"/>
       <c r="G49" s="46"/>
@@ -3141,11 +3218,11 @@
       <c r="A50" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="113"/>
-      <c r="D50" s="114"/>
+      <c r="B50" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="117"/>
+      <c r="D50" s="118"/>
       <c r="E50" s="48"/>
       <c r="F50" s="49"/>
       <c r="G50" s="50"/>
@@ -3163,11 +3240,15 @@
       <c r="A51" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="116"/>
-      <c r="D51" s="117"/>
+      <c r="B51" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E51" s="7"/>
       <c r="F51" s="52"/>
       <c r="G51" s="46"/>
@@ -3185,11 +3266,11 @@
       <c r="A52" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B52" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="114"/>
+      <c r="B52" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="117"/>
+      <c r="D52" s="118"/>
       <c r="E52" s="48"/>
       <c r="F52" s="49"/>
       <c r="G52" s="50"/>
@@ -3207,11 +3288,15 @@
       <c r="A53" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="116"/>
-      <c r="D53" s="117"/>
+      <c r="B53" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E53" s="51"/>
       <c r="F53" s="45"/>
       <c r="G53" s="46"/>
@@ -3229,11 +3314,11 @@
       <c r="A54" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="113"/>
-      <c r="D54" s="114"/>
+      <c r="B54" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="117"/>
+      <c r="D54" s="118"/>
       <c r="E54" s="48"/>
       <c r="F54" s="49"/>
       <c r="G54" s="50"/>
@@ -3251,11 +3336,15 @@
       <c r="A55" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="116"/>
-      <c r="D55" s="117"/>
+      <c r="B55" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E55" s="51"/>
       <c r="F55" s="45"/>
       <c r="G55" s="46"/>
@@ -3273,11 +3362,11 @@
       <c r="A56" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C56" s="113"/>
-      <c r="D56" s="114"/>
+      <c r="B56" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="117"/>
+      <c r="D56" s="118"/>
       <c r="E56" s="48"/>
       <c r="F56" s="49"/>
       <c r="G56" s="50"/>
@@ -3295,11 +3384,15 @@
       <c r="A57" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B57" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" s="116"/>
-      <c r="D57" s="117"/>
+      <c r="B57" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E57" s="51"/>
       <c r="F57" s="45"/>
       <c r="G57" s="46"/>
@@ -3317,21 +3410,21 @@
       <c r="A58" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="182"/>
-      <c r="C58" s="119"/>
-      <c r="D58" s="120"/>
+      <c r="B58" s="131"/>
+      <c r="C58" s="132"/>
+      <c r="D58" s="133"/>
       <c r="E58" s="53"/>
       <c r="F58" s="54"/>
-      <c r="G58" s="181" t="s">
+      <c r="G58" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="H58" s="119"/>
-      <c r="I58" s="119"/>
-      <c r="J58" s="119"/>
-      <c r="K58" s="119"/>
-      <c r="L58" s="119"/>
-      <c r="M58" s="119"/>
-      <c r="N58" s="119"/>
+      <c r="H58" s="132"/>
+      <c r="I58" s="132"/>
+      <c r="J58" s="132"/>
+      <c r="K58" s="132"/>
+      <c r="L58" s="132"/>
+      <c r="M58" s="132"/>
+      <c r="N58" s="132"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
     </row>
@@ -3339,11 +3432,11 @@
       <c r="A59" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="113"/>
-      <c r="D59" s="114"/>
+      <c r="B59" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="117"/>
+      <c r="D59" s="118"/>
       <c r="E59" s="48"/>
       <c r="F59" s="49"/>
       <c r="G59" s="50"/>
@@ -3361,11 +3454,15 @@
       <c r="A60" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="116"/>
-      <c r="D60" s="117"/>
+      <c r="B60" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E60" s="51"/>
       <c r="F60" s="45"/>
       <c r="G60" s="46"/>
@@ -3383,11 +3480,11 @@
       <c r="A61" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" s="113"/>
-      <c r="D61" s="114"/>
+      <c r="B61" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="117"/>
+      <c r="D61" s="118"/>
       <c r="E61" s="48"/>
       <c r="F61" s="49"/>
       <c r="G61" s="50"/>
@@ -3405,11 +3502,15 @@
       <c r="A62" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C62" s="116"/>
-      <c r="D62" s="117"/>
+      <c r="B62" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E62" s="51"/>
       <c r="F62" s="45"/>
       <c r="G62" s="46"/>
@@ -3427,11 +3528,11 @@
       <c r="A63" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B63" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="113"/>
-      <c r="D63" s="114"/>
+      <c r="B63" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="117"/>
+      <c r="D63" s="118"/>
       <c r="E63" s="48"/>
       <c r="F63" s="49"/>
       <c r="G63" s="50"/>
@@ -3449,11 +3550,15 @@
       <c r="A64" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B64" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="116"/>
-      <c r="D64" s="117"/>
+      <c r="B64" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E64" s="51"/>
       <c r="F64" s="45"/>
       <c r="G64" s="46"/>
@@ -3471,11 +3576,11 @@
       <c r="A65" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="113"/>
-      <c r="D65" s="114"/>
+      <c r="B65" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="117"/>
+      <c r="D65" s="118"/>
       <c r="E65" s="48"/>
       <c r="F65" s="49"/>
       <c r="G65" s="50"/>
@@ -3493,11 +3598,15 @@
       <c r="A66" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="116"/>
-      <c r="D66" s="117"/>
+      <c r="B66" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E66" s="51"/>
       <c r="F66" s="45"/>
       <c r="G66" s="46"/>
@@ -3515,11 +3624,11 @@
       <c r="A67" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67" s="113"/>
-      <c r="D67" s="114"/>
+      <c r="B67" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="117"/>
+      <c r="D67" s="118"/>
       <c r="E67" s="48"/>
       <c r="F67" s="49"/>
       <c r="G67" s="50"/>
@@ -3537,11 +3646,15 @@
       <c r="A68" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C68" s="116"/>
-      <c r="D68" s="117"/>
+      <c r="B68" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E68" s="51"/>
       <c r="F68" s="45"/>
       <c r="G68" s="46"/>
@@ -3559,11 +3672,11 @@
       <c r="A69" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="113"/>
-      <c r="D69" s="114"/>
+      <c r="B69" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="117"/>
+      <c r="D69" s="118"/>
       <c r="E69" s="48"/>
       <c r="F69" s="49"/>
       <c r="G69" s="50"/>
@@ -3581,11 +3694,15 @@
       <c r="A70" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="116"/>
-      <c r="D70" s="117"/>
+      <c r="B70" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C70" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E70" s="51"/>
       <c r="F70" s="45"/>
       <c r="G70" s="46"/>
@@ -3603,11 +3720,11 @@
       <c r="A71" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="113"/>
-      <c r="D71" s="114"/>
+      <c r="B71" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" s="117"/>
+      <c r="D71" s="118"/>
       <c r="E71" s="48"/>
       <c r="F71" s="49"/>
       <c r="G71" s="50"/>
@@ -3625,11 +3742,15 @@
       <c r="A72" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="116"/>
-      <c r="D72" s="117"/>
+      <c r="B72" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D72" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E72" s="51"/>
       <c r="F72" s="45"/>
       <c r="G72" s="46"/>
@@ -3647,11 +3768,11 @@
       <c r="A73" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" s="113"/>
-      <c r="D73" s="114"/>
+      <c r="B73" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C73" s="117"/>
+      <c r="D73" s="118"/>
       <c r="E73" s="48"/>
       <c r="F73" s="49"/>
       <c r="G73" s="50"/>
@@ -3669,11 +3790,15 @@
       <c r="A74" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="116"/>
-      <c r="D74" s="117"/>
+      <c r="B74" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D74" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E74" s="51"/>
       <c r="F74" s="45"/>
       <c r="G74" s="46"/>
@@ -3691,11 +3816,11 @@
       <c r="A75" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="113"/>
-      <c r="D75" s="114"/>
+      <c r="B75" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="117"/>
+      <c r="D75" s="118"/>
       <c r="E75" s="48"/>
       <c r="F75" s="49"/>
       <c r="G75" s="50"/>
@@ -3713,11 +3838,15 @@
       <c r="A76" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" s="116"/>
-      <c r="D76" s="117"/>
+      <c r="B76" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C76" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E76" s="51"/>
       <c r="F76" s="45"/>
       <c r="G76" s="46"/>
@@ -3735,11 +3864,11 @@
       <c r="A77" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77" s="113"/>
-      <c r="D77" s="114"/>
+      <c r="B77" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="117"/>
+      <c r="D77" s="118"/>
       <c r="E77" s="48"/>
       <c r="F77" s="49"/>
       <c r="G77" s="50"/>
@@ -3757,11 +3886,15 @@
       <c r="A78" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" s="116"/>
-      <c r="D78" s="117"/>
+      <c r="B78" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E78" s="51"/>
       <c r="F78" s="45"/>
       <c r="G78" s="46"/>
@@ -3779,11 +3912,11 @@
       <c r="A79" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="113"/>
-      <c r="D79" s="114"/>
+      <c r="B79" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="117"/>
+      <c r="D79" s="118"/>
       <c r="E79" s="48"/>
       <c r="F79" s="49"/>
       <c r="G79" s="50"/>
@@ -3801,11 +3934,15 @@
       <c r="A80" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B80" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C80" s="116"/>
-      <c r="D80" s="117"/>
+      <c r="B80" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C80" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E80" s="51"/>
       <c r="F80" s="45"/>
       <c r="G80" s="46"/>
@@ -3823,11 +3960,11 @@
       <c r="A81" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B81" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="113"/>
-      <c r="D81" s="114"/>
+      <c r="B81" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" s="117"/>
+      <c r="D81" s="118"/>
       <c r="E81" s="48"/>
       <c r="F81" s="49"/>
       <c r="G81" s="50"/>
@@ -3845,11 +3982,15 @@
       <c r="A82" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B82" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C82" s="116"/>
-      <c r="D82" s="117"/>
+      <c r="B82" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E82" s="51"/>
       <c r="F82" s="45"/>
       <c r="G82" s="46"/>
@@ -3867,11 +4008,11 @@
       <c r="A83" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C83" s="113"/>
-      <c r="D83" s="114"/>
+      <c r="B83" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="117"/>
+      <c r="D83" s="118"/>
       <c r="E83" s="48"/>
       <c r="F83" s="49"/>
       <c r="G83" s="50"/>
@@ -3889,11 +4030,15 @@
       <c r="A84" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B84" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C84" s="116"/>
-      <c r="D84" s="117"/>
+      <c r="B84" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C84" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D84" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E84" s="51"/>
       <c r="F84" s="45"/>
       <c r="G84" s="46"/>
@@ -3911,11 +4056,11 @@
       <c r="A85" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B85" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C85" s="113"/>
-      <c r="D85" s="114"/>
+      <c r="B85" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="117"/>
+      <c r="D85" s="118"/>
       <c r="E85" s="48"/>
       <c r="F85" s="49"/>
       <c r="G85" s="50"/>
@@ -3933,11 +4078,15 @@
       <c r="A86" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B86" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C86" s="116"/>
-      <c r="D86" s="117"/>
+      <c r="B86" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E86" s="51"/>
       <c r="F86" s="45"/>
       <c r="G86" s="46"/>
@@ -3955,11 +4104,11 @@
       <c r="A87" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B87" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87" s="113"/>
-      <c r="D87" s="114"/>
+      <c r="B87" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="117"/>
+      <c r="D87" s="118"/>
       <c r="E87" s="48"/>
       <c r="F87" s="49"/>
       <c r="G87" s="50"/>
@@ -3977,11 +4126,15 @@
       <c r="A88" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B88" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C88" s="116"/>
-      <c r="D88" s="117"/>
+      <c r="B88" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C88" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D88" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E88" s="51"/>
       <c r="F88" s="45"/>
       <c r="G88" s="46"/>
@@ -3999,11 +4152,11 @@
       <c r="A89" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B89" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C89" s="113"/>
-      <c r="D89" s="114"/>
+      <c r="B89" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89" s="117"/>
+      <c r="D89" s="118"/>
       <c r="E89" s="48"/>
       <c r="F89" s="49"/>
       <c r="G89" s="50"/>
@@ -4021,11 +4174,15 @@
       <c r="A90" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B90" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C90" s="116"/>
-      <c r="D90" s="117"/>
+      <c r="B90" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D90" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E90" s="51"/>
       <c r="F90" s="45"/>
       <c r="G90" s="46"/>
@@ -4043,11 +4200,11 @@
       <c r="A91" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C91" s="113"/>
-      <c r="D91" s="114"/>
+      <c r="B91" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="117"/>
+      <c r="D91" s="118"/>
       <c r="E91" s="48"/>
       <c r="F91" s="49"/>
       <c r="G91" s="50"/>
@@ -4065,11 +4222,15 @@
       <c r="A92" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C92" s="116"/>
-      <c r="D92" s="117"/>
+      <c r="B92" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D92" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E92" s="51"/>
       <c r="F92" s="45"/>
       <c r="G92" s="46"/>
@@ -4087,11 +4248,11 @@
       <c r="A93" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C93" s="113"/>
-      <c r="D93" s="114"/>
+      <c r="B93" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="117"/>
+      <c r="D93" s="118"/>
       <c r="E93" s="48"/>
       <c r="F93" s="49"/>
       <c r="G93" s="50"/>
@@ -4109,11 +4270,15 @@
       <c r="A94" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C94" s="116"/>
-      <c r="D94" s="117"/>
+      <c r="B94" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C94" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E94" s="51"/>
       <c r="F94" s="45"/>
       <c r="G94" s="46"/>
@@ -4131,11 +4296,11 @@
       <c r="A95" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B95" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C95" s="113"/>
-      <c r="D95" s="114"/>
+      <c r="B95" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95" s="117"/>
+      <c r="D95" s="118"/>
       <c r="E95" s="48"/>
       <c r="F95" s="49"/>
       <c r="G95" s="50"/>
@@ -4153,11 +4318,15 @@
       <c r="A96" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B96" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" s="116"/>
-      <c r="D96" s="117"/>
+      <c r="B96" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C96" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D96" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E96" s="51"/>
       <c r="F96" s="45"/>
       <c r="G96" s="46"/>
@@ -4175,11 +4344,11 @@
       <c r="A97" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B97" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C97" s="113"/>
-      <c r="D97" s="114"/>
+      <c r="B97" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97" s="117"/>
+      <c r="D97" s="118"/>
       <c r="E97" s="48"/>
       <c r="F97" s="49"/>
       <c r="G97" s="50"/>
@@ -4197,11 +4366,15 @@
       <c r="A98" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B98" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C98" s="116"/>
-      <c r="D98" s="117"/>
+      <c r="B98" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C98" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D98" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E98" s="51"/>
       <c r="F98" s="45"/>
       <c r="G98" s="46"/>
@@ -4219,11 +4392,11 @@
       <c r="A99" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B99" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C99" s="113"/>
-      <c r="D99" s="114"/>
+      <c r="B99" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99" s="117"/>
+      <c r="D99" s="118"/>
       <c r="E99" s="48"/>
       <c r="F99" s="49"/>
       <c r="G99" s="50"/>
@@ -4241,11 +4414,15 @@
       <c r="A100" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B100" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C100" s="116"/>
-      <c r="D100" s="117"/>
+      <c r="B100" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C100" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D100" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E100" s="51"/>
       <c r="F100" s="45"/>
       <c r="G100" s="46"/>
@@ -4263,11 +4440,11 @@
       <c r="A101" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="B101" s="112" t="s">
-        <v>72</v>
-      </c>
-      <c r="C101" s="113"/>
-      <c r="D101" s="114"/>
+      <c r="B101" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="C101" s="117"/>
+      <c r="D101" s="118"/>
       <c r="E101" s="48"/>
       <c r="F101" s="49"/>
       <c r="G101" s="50"/>
@@ -4285,11 +4462,15 @@
       <c r="A102" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B102" s="115" t="s">
-        <v>75</v>
-      </c>
-      <c r="C102" s="116"/>
-      <c r="D102" s="117"/>
+      <c r="B102" s="219" t="s">
+        <v>109</v>
+      </c>
+      <c r="C102" s="220" t="s">
+        <v>110</v>
+      </c>
+      <c r="D102" s="221" t="s">
+        <v>112</v>
+      </c>
       <c r="E102" s="51"/>
       <c r="F102" s="45"/>
       <c r="G102" s="46"/>
@@ -4484,78 +4665,41 @@
       <c r="P112" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B26:F27"/>
-    <mergeCell ref="G26:P27"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="G58:N58"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
+  <mergeCells count="82">
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:P25"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:P10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G13:P13"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="G22:P22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:P24"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C14:P14"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:P17"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="J6:K6"/>
@@ -4567,44 +4711,46 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="M8:P8"/>
     <mergeCell ref="J7:M7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:P10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G13:P13"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:P22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:P19"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="C14:P14"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="G58:N58"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B26:F27"/>
+    <mergeCell ref="G26:P27"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B67:D67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4612,7 +4758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE54FB90-7D9E-467C-8724-1EBEEF7A282C}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
@@ -4642,11 +4788,11 @@
       <c r="A4" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="198" t="s">
+      <c r="B4" s="204" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="199"/>
-      <c r="D4" s="200"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
       <c r="E4" s="84"/>
       <c r="F4" s="83" t="s">
         <v>85</v>
@@ -4659,11 +4805,11 @@
       <c r="A5" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="201" t="s">
+      <c r="B5" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="202"/>
-      <c r="D5" s="203"/>
+      <c r="C5" s="208"/>
+      <c r="D5" s="209"/>
       <c r="E5" s="84"/>
       <c r="F5" s="87" t="s">
         <v>87</v>
@@ -4676,11 +4822,11 @@
       <c r="A6" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="204" t="s">
+      <c r="B6" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="205"/>
-      <c r="D6" s="206"/>
+      <c r="C6" s="211"/>
+      <c r="D6" s="212"/>
       <c r="E6" s="84"/>
       <c r="F6" s="90" t="s">
         <v>90</v>
@@ -4693,11 +4839,11 @@
       <c r="A7" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="207" t="s">
+      <c r="B7" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="208"/>
-      <c r="D7" s="209"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="215"/>
       <c r="E7" s="84"/>
       <c r="F7" s="93" t="s">
         <v>93</v>
@@ -4710,41 +4856,41 @@
       <c r="A8" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="210" t="s">
+      <c r="B8" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="211"/>
-      <c r="D8" s="212"/>
+      <c r="C8" s="217"/>
+      <c r="D8" s="218"/>
       <c r="E8" s="84"/>
       <c r="F8" s="96"/>
-      <c r="G8" s="191"/>
+      <c r="G8" s="197"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="194" t="s">
+      <c r="B9" s="200" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="195"/>
-      <c r="D9" s="196"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="202"/>
       <c r="E9" s="84"/>
       <c r="F9" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="192"/>
+      <c r="G9" s="198"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="197" t="s">
+      <c r="B10" s="203" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="195"/>
-      <c r="D10" s="196"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="202"/>
       <c r="F10" s="100"/>
-      <c r="G10" s="193"/>
+      <c r="G10" s="199"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="101"/>
@@ -4778,542 +4924,569 @@
       <c r="A13" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="213" t="s">
+      <c r="B13" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="214"/>
-      <c r="D13" s="214"/>
-      <c r="E13" s="214"/>
-      <c r="F13" s="215"/>
+      <c r="C13" s="195"/>
+      <c r="D13" s="195"/>
+      <c r="E13" s="195"/>
+      <c r="F13" s="196"/>
       <c r="G13" s="107"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="213" t="s">
+      <c r="B14" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="214"/>
-      <c r="D14" s="214"/>
-      <c r="E14" s="214"/>
-      <c r="F14" s="215"/>
+      <c r="C14" s="195"/>
+      <c r="D14" s="195"/>
+      <c r="E14" s="195"/>
+      <c r="F14" s="196"/>
       <c r="G14" s="108"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="213" t="s">
+      <c r="B15" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="214"/>
-      <c r="D15" s="214"/>
-      <c r="E15" s="214"/>
-      <c r="F15" s="215"/>
+      <c r="C15" s="195"/>
+      <c r="D15" s="195"/>
+      <c r="E15" s="195"/>
+      <c r="F15" s="196"/>
       <c r="G15" s="110"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="213" t="s">
+      <c r="B16" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
-      <c r="E16" s="214"/>
-      <c r="F16" s="215"/>
+      <c r="C16" s="195"/>
+      <c r="D16" s="195"/>
+      <c r="E16" s="195"/>
+      <c r="F16" s="196"/>
       <c r="G16" s="110"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="213" t="s">
+      <c r="B17" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="214"/>
-      <c r="D17" s="214"/>
-      <c r="E17" s="214"/>
-      <c r="F17" s="215"/>
+      <c r="C17" s="195"/>
+      <c r="D17" s="195"/>
+      <c r="E17" s="195"/>
+      <c r="F17" s="196"/>
       <c r="G17" s="110"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="213" t="s">
+      <c r="B18" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="214"/>
-      <c r="F18" s="215"/>
+      <c r="C18" s="195"/>
+      <c r="D18" s="195"/>
+      <c r="E18" s="195"/>
+      <c r="F18" s="196"/>
       <c r="G18" s="110"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="213" t="s">
+      <c r="B19" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="214"/>
-      <c r="D19" s="214"/>
-      <c r="E19" s="214"/>
-      <c r="F19" s="215"/>
+      <c r="C19" s="195"/>
+      <c r="D19" s="195"/>
+      <c r="E19" s="195"/>
+      <c r="F19" s="196"/>
       <c r="G19" s="110"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="213" t="s">
+      <c r="B20" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="214"/>
-      <c r="D20" s="214"/>
-      <c r="E20" s="214"/>
-      <c r="F20" s="215"/>
+      <c r="C20" s="195"/>
+      <c r="D20" s="195"/>
+      <c r="E20" s="195"/>
+      <c r="F20" s="196"/>
       <c r="G20" s="110"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="213" t="s">
+      <c r="B21" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="214"/>
-      <c r="D21" s="214"/>
-      <c r="E21" s="214"/>
-      <c r="F21" s="215"/>
+      <c r="C21" s="195"/>
+      <c r="D21" s="195"/>
+      <c r="E21" s="195"/>
+      <c r="F21" s="196"/>
       <c r="G21" s="110"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="213" t="s">
+      <c r="B22" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="214"/>
-      <c r="D22" s="214"/>
-      <c r="E22" s="214"/>
-      <c r="F22" s="215"/>
+      <c r="C22" s="195"/>
+      <c r="D22" s="195"/>
+      <c r="E22" s="195"/>
+      <c r="F22" s="196"/>
       <c r="G22" s="110"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="213" t="s">
+      <c r="B23" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="214"/>
-      <c r="D23" s="214"/>
-      <c r="E23" s="214"/>
-      <c r="F23" s="215"/>
+      <c r="C23" s="195"/>
+      <c r="D23" s="195"/>
+      <c r="E23" s="195"/>
+      <c r="F23" s="196"/>
       <c r="G23" s="110"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="213" t="s">
+      <c r="B24" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="214"/>
-      <c r="D24" s="214"/>
-      <c r="E24" s="214"/>
-      <c r="F24" s="215"/>
+      <c r="C24" s="195"/>
+      <c r="D24" s="195"/>
+      <c r="E24" s="195"/>
+      <c r="F24" s="196"/>
       <c r="G24" s="109"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="213" t="s">
+      <c r="B25" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="214"/>
-      <c r="D25" s="214"/>
-      <c r="E25" s="214"/>
-      <c r="F25" s="215"/>
+      <c r="C25" s="195"/>
+      <c r="D25" s="195"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="196"/>
       <c r="G25" s="109"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="213" t="s">
+      <c r="B26" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="214"/>
-      <c r="D26" s="214"/>
-      <c r="E26" s="214"/>
-      <c r="F26" s="215"/>
+      <c r="C26" s="195"/>
+      <c r="D26" s="195"/>
+      <c r="E26" s="195"/>
+      <c r="F26" s="196"/>
       <c r="G26" s="109"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="213" t="s">
+      <c r="B27" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="214"/>
-      <c r="D27" s="214"/>
-      <c r="E27" s="214"/>
-      <c r="F27" s="215"/>
+      <c r="C27" s="195"/>
+      <c r="D27" s="195"/>
+      <c r="E27" s="195"/>
+      <c r="F27" s="196"/>
       <c r="G27" s="109"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="213" t="s">
+      <c r="B28" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="214"/>
-      <c r="D28" s="214"/>
-      <c r="E28" s="214"/>
-      <c r="F28" s="215"/>
+      <c r="C28" s="195"/>
+      <c r="D28" s="195"/>
+      <c r="E28" s="195"/>
+      <c r="F28" s="196"/>
       <c r="G28" s="109"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="213" t="s">
+      <c r="B29" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="214"/>
-      <c r="D29" s="214"/>
-      <c r="E29" s="214"/>
-      <c r="F29" s="215"/>
+      <c r="C29" s="195"/>
+      <c r="D29" s="195"/>
+      <c r="E29" s="195"/>
+      <c r="F29" s="196"/>
       <c r="G29" s="109"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="213" t="s">
+      <c r="B30" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="214"/>
-      <c r="D30" s="214"/>
-      <c r="E30" s="214"/>
-      <c r="F30" s="215"/>
+      <c r="C30" s="195"/>
+      <c r="D30" s="195"/>
+      <c r="E30" s="195"/>
+      <c r="F30" s="196"/>
       <c r="G30" s="109"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="213" t="s">
+      <c r="B31" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="214"/>
-      <c r="D31" s="214"/>
-      <c r="E31" s="214"/>
-      <c r="F31" s="215"/>
+      <c r="C31" s="195"/>
+      <c r="D31" s="195"/>
+      <c r="E31" s="195"/>
+      <c r="F31" s="196"/>
       <c r="G31" s="109"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="213" t="s">
+      <c r="B32" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="214"/>
-      <c r="D32" s="214"/>
-      <c r="E32" s="214"/>
-      <c r="F32" s="215"/>
+      <c r="C32" s="195"/>
+      <c r="D32" s="195"/>
+      <c r="E32" s="195"/>
+      <c r="F32" s="196"/>
       <c r="G32" s="109"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="213" t="s">
+      <c r="B33" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="214"/>
-      <c r="D33" s="214"/>
-      <c r="E33" s="214"/>
-      <c r="F33" s="215"/>
+      <c r="C33" s="195"/>
+      <c r="D33" s="195"/>
+      <c r="E33" s="195"/>
+      <c r="F33" s="196"/>
       <c r="G33" s="109"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="213" t="s">
+      <c r="B34" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="214"/>
-      <c r="D34" s="214"/>
-      <c r="E34" s="214"/>
-      <c r="F34" s="215"/>
+      <c r="C34" s="195"/>
+      <c r="D34" s="195"/>
+      <c r="E34" s="195"/>
+      <c r="F34" s="196"/>
       <c r="G34" s="109"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="213" t="s">
+      <c r="B35" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="214"/>
-      <c r="D35" s="214"/>
-      <c r="E35" s="214"/>
-      <c r="F35" s="215"/>
+      <c r="C35" s="195"/>
+      <c r="D35" s="195"/>
+      <c r="E35" s="195"/>
+      <c r="F35" s="196"/>
       <c r="G35" s="109"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="213" t="s">
+      <c r="B36" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="214"/>
-      <c r="D36" s="214"/>
-      <c r="E36" s="214"/>
-      <c r="F36" s="215"/>
+      <c r="C36" s="195"/>
+      <c r="D36" s="195"/>
+      <c r="E36" s="195"/>
+      <c r="F36" s="196"/>
       <c r="G36" s="109"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="213" t="s">
+      <c r="B37" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="214"/>
-      <c r="D37" s="214"/>
-      <c r="E37" s="214"/>
-      <c r="F37" s="215"/>
+      <c r="C37" s="195"/>
+      <c r="D37" s="195"/>
+      <c r="E37" s="195"/>
+      <c r="F37" s="196"/>
       <c r="G37" s="109"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="213" t="s">
+      <c r="B38" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="214"/>
-      <c r="D38" s="214"/>
-      <c r="E38" s="214"/>
-      <c r="F38" s="215"/>
+      <c r="C38" s="195"/>
+      <c r="D38" s="195"/>
+      <c r="E38" s="195"/>
+      <c r="F38" s="196"/>
       <c r="G38" s="109"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="213" t="s">
+      <c r="B39" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="214"/>
-      <c r="D39" s="214"/>
-      <c r="E39" s="214"/>
-      <c r="F39" s="215"/>
+      <c r="C39" s="195"/>
+      <c r="D39" s="195"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="196"/>
       <c r="G39" s="109"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="213" t="s">
+      <c r="B40" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="214"/>
-      <c r="D40" s="214"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="215"/>
+      <c r="C40" s="195"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="195"/>
+      <c r="F40" s="196"/>
       <c r="G40" s="109"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="213" t="s">
+      <c r="B41" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="214"/>
-      <c r="D41" s="214"/>
-      <c r="E41" s="214"/>
-      <c r="F41" s="215"/>
+      <c r="C41" s="195"/>
+      <c r="D41" s="195"/>
+      <c r="E41" s="195"/>
+      <c r="F41" s="196"/>
       <c r="G41" s="109"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="213" t="s">
+      <c r="B42" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="214"/>
-      <c r="D42" s="214"/>
-      <c r="E42" s="214"/>
-      <c r="F42" s="215"/>
+      <c r="C42" s="195"/>
+      <c r="D42" s="195"/>
+      <c r="E42" s="195"/>
+      <c r="F42" s="196"/>
       <c r="G42" s="109"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="213" t="s">
+      <c r="B43" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="214"/>
-      <c r="D43" s="214"/>
-      <c r="E43" s="214"/>
-      <c r="F43" s="215"/>
+      <c r="C43" s="195"/>
+      <c r="D43" s="195"/>
+      <c r="E43" s="195"/>
+      <c r="F43" s="196"/>
       <c r="G43" s="109"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="213" t="s">
+      <c r="B44" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="214"/>
-      <c r="D44" s="214"/>
-      <c r="E44" s="214"/>
-      <c r="F44" s="215"/>
+      <c r="C44" s="195"/>
+      <c r="D44" s="195"/>
+      <c r="E44" s="195"/>
+      <c r="F44" s="196"/>
       <c r="G44" s="109"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="213" t="s">
+      <c r="B45" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="214"/>
-      <c r="D45" s="214"/>
-      <c r="E45" s="214"/>
-      <c r="F45" s="215"/>
+      <c r="C45" s="195"/>
+      <c r="D45" s="195"/>
+      <c r="E45" s="195"/>
+      <c r="F45" s="196"/>
       <c r="G45" s="109"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="213" t="s">
+      <c r="B46" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="214"/>
-      <c r="D46" s="214"/>
-      <c r="E46" s="214"/>
-      <c r="F46" s="215"/>
+      <c r="C46" s="195"/>
+      <c r="D46" s="195"/>
+      <c r="E46" s="195"/>
+      <c r="F46" s="196"/>
       <c r="G46" s="109"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="213" t="s">
+      <c r="B47" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="214"/>
-      <c r="D47" s="214"/>
-      <c r="E47" s="214"/>
-      <c r="F47" s="215"/>
+      <c r="C47" s="195"/>
+      <c r="D47" s="195"/>
+      <c r="E47" s="195"/>
+      <c r="F47" s="196"/>
       <c r="G47" s="109"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="213" t="s">
+      <c r="B48" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="214"/>
-      <c r="D48" s="214"/>
-      <c r="E48" s="214"/>
-      <c r="F48" s="215"/>
+      <c r="C48" s="195"/>
+      <c r="D48" s="195"/>
+      <c r="E48" s="195"/>
+      <c r="F48" s="196"/>
       <c r="G48" s="109"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="213" t="s">
+      <c r="B49" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="214"/>
-      <c r="D49" s="214"/>
-      <c r="E49" s="214"/>
-      <c r="F49" s="215"/>
+      <c r="C49" s="195"/>
+      <c r="D49" s="195"/>
+      <c r="E49" s="195"/>
+      <c r="F49" s="196"/>
       <c r="G49" s="109"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="213" t="s">
+      <c r="B50" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="214"/>
-      <c r="D50" s="214"/>
-      <c r="E50" s="214"/>
-      <c r="F50" s="215"/>
+      <c r="C50" s="195"/>
+      <c r="D50" s="195"/>
+      <c r="E50" s="195"/>
+      <c r="F50" s="196"/>
       <c r="G50" s="109"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B51" s="213" t="s">
+      <c r="B51" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="214"/>
-      <c r="D51" s="214"/>
-      <c r="E51" s="214"/>
-      <c r="F51" s="215"/>
+      <c r="C51" s="195"/>
+      <c r="D51" s="195"/>
+      <c r="E51" s="195"/>
+      <c r="F51" s="196"/>
       <c r="G51" s="109"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="213" t="s">
+      <c r="B52" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="214"/>
-      <c r="D52" s="214"/>
-      <c r="E52" s="214"/>
-      <c r="F52" s="215"/>
+      <c r="C52" s="195"/>
+      <c r="D52" s="195"/>
+      <c r="E52" s="195"/>
+      <c r="F52" s="196"/>
       <c r="G52" s="109"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="213" t="s">
+      <c r="B53" s="194" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="214"/>
-      <c r="D53" s="214"/>
-      <c r="E53" s="214"/>
-      <c r="F53" s="215"/>
+      <c r="C53" s="195"/>
+      <c r="D53" s="195"/>
+      <c r="E53" s="195"/>
+      <c r="F53" s="196"/>
       <c r="G53" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="B48:F48"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
@@ -5326,38 +5499,11 @@
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>